<commit_message>
finalized data import script to put everything in cshl.all
</commit_message>
<xml_diff>
--- a/140803_rgv2_and_dilutions.xlsx
+++ b/140803_rgv2_and_dilutions.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="21405"/>
   <workbookPr autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="140" windowWidth="17240" windowHeight="6980" activeTab="2"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="15480" activeTab="5"/>
   </bookViews>
   <sheets>
     <sheet name="blanks2" sheetId="9" r:id="rId1"/>
@@ -1131,7 +1131,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1159,6 +1159,22 @@
       <color indexed="81"/>
       <name val="Tahoma"/>
       <charset val="1"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="10">
@@ -1226,7 +1242,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="8">
+  <cellStyleXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0"/>
@@ -1235,6 +1251,8 @@
     <xf numFmtId="0" fontId="2" fillId="6" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1244,7 +1262,9 @@
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="8">
+  <cellStyles count="10">
+    <cellStyle name="Followed Hyperlink" xfId="9" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="8" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Tecan.At.Excel.Attenuation" xfId="6"/>
     <cellStyle name="Tecan.At.Excel.AutoGain_0" xfId="7"/>
@@ -2563,7 +2583,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D69" sqref="D69"/>
     </sheetView>
   </sheetViews>
@@ -3639,7 +3659,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView topLeftCell="A52" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
@@ -4713,7 +4733,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M70"/>
   <sheetViews>
-    <sheetView topLeftCell="A49" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A14" sqref="A14:XFD16"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <sheetData>
@@ -5774,6 +5796,7 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <legacyDrawing r:id="rId1"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
@@ -5787,8 +5810,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:M67"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D20" sqref="D20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C26" sqref="C26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>